<commit_message>
Clase 27 de noviembre: laberinto con matrices
</commit_message>
<xml_diff>
--- a/Semana 7/Laberinto.xlsx
+++ b/Semana 7/Laberinto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claudiacortes/Desktop/P1 Q4 2025/Semana 7/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7156FF5-1412-1E43-9D8A-288A80C1EC3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B00930FE-33CE-784B-A6C0-3AA3C18262F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{BFC22E4C-E588-0C49-87BC-600B986A7285}"/>
   </bookViews>
@@ -35,12 +35,72 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
   <si>
     <t>*</t>
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>3,2</t>
+  </si>
+  <si>
+    <t>3,1</t>
+  </si>
+  <si>
+    <t>izquierda</t>
+  </si>
+  <si>
+    <t>derecha</t>
+  </si>
+  <si>
+    <t>3,3</t>
+  </si>
+  <si>
+    <t>col</t>
+  </si>
+  <si>
+    <t>arriba</t>
+  </si>
+  <si>
+    <t>abajo</t>
+  </si>
+  <si>
+    <t>2,2</t>
+  </si>
+  <si>
+    <t>4,2</t>
+  </si>
+  <si>
+    <t>fila,columna</t>
+  </si>
+  <si>
+    <t>fila</t>
+  </si>
+  <si>
+    <t xml:space="preserve">columna 0 </t>
+  </si>
+  <si>
+    <t>no movimientos a la izq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fila 0 </t>
+  </si>
+  <si>
+    <t>no movimientos arriba</t>
+  </si>
+  <si>
+    <t>columna 4</t>
+  </si>
+  <si>
+    <t>no movimientos a la derecha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fila 4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">no movimientos hacia abajo </t>
   </si>
 </sst>
 </file>
@@ -56,7 +116,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -69,8 +129,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -93,11 +165,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -106,6 +187,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -422,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC15E7B7-D3BF-8041-9BAA-DF090485EB8E}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="H4" sqref="H4:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -437,7 +533,7 @@
     <col min="6" max="6" width="5.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1">
         <v>0</v>
@@ -451,8 +547,11 @@
       <c r="E1" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F1" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -460,8 +559,9 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -469,8 +569,9 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -478,8 +579,15 @@
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F4" s="2"/>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -487,8 +595,15 @@
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F5" s="2"/>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -496,8 +611,23 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F6" s="2"/>
+      <c r="H6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1">
         <v>0</v>
@@ -515,11 +645,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>0</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="5"/>
       <c r="C9" s="3" t="s">
         <v>0</v>
       </c>
@@ -533,19 +663,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>1</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="4"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>2</v>
       </c>
@@ -560,26 +693,50 @@
       <c r="F11" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H11" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" t="s">
+        <v>5</v>
+      </c>
+      <c r="J11" t="s">
+        <v>8</v>
+      </c>
+      <c r="K11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>3</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="C12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H12" t="s">
+        <v>2</v>
+      </c>
+      <c r="I12" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" t="s">
+        <v>2</v>
+      </c>
+      <c r="K12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>4</v>
       </c>
@@ -598,8 +755,49 @@
       <c r="F13" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="H13" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J13" t="s">
+        <v>10</v>
+      </c>
+      <c r="K13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" t="s">
+        <v>7</v>
+      </c>
+      <c r="J14" t="s">
+        <v>13</v>
+      </c>
+      <c r="K14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H15">
+        <v>-1</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>-1</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>